<commit_message>
Update time sheet - ranjith
</commit_message>
<xml_diff>
--- a/Aurora/Process/PTW-Timesheet.xlsx
+++ b/Aurora/Process/PTW-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aspire-Team Aurora project\Project\Aurora\Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7253B17D-4B08-45E4-8E40-2960E32FA98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95E970A9-671B-4671-AAF5-080E65119C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="44" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="247">
   <si>
     <t>Resource Name</t>
   </si>
@@ -876,6 +876,20 @@
   </si>
   <si>
     <t>2.25 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.00-9.15 -Brainstorming with team
+9.30-10.30-NFR
+10.30-10.45-break
+10.45-12.00-learnt about what is API codefirst uproch 
+12.00-12.30-learnt about HTTP(put,update,delete,get)
+12.30-1.00-Discussion with the team before meeting
+1.00-1.30-Lunch
+1.30-2.45-Review session with rafi
+3.00-4.00-Timesheet and SVN Session
+4.30-5.00-Discussion with team after the review meeting 
+5.00-5.30-Data model 
+</t>
   </si>
 </sst>
 </file>
@@ -2470,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C081B83-E4F9-48C7-866F-0458E5F9EE36}">
   <dimension ref="E7:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -2811,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AF63B3-2472-435F-A833-BA0C49A1E3BE}">
   <dimension ref="E7:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2997,7 +3011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="5:11" ht="121.5" customHeight="1">
+    <row r="18" spans="5:11" ht="96.75" customHeight="1">
       <c r="E18" s="27" t="s">
         <v>14</v>
       </c>
@@ -3012,12 +3026,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="5:11" ht="85.5" customHeight="1">
+    <row r="19" spans="5:11" ht="223.5" customHeight="1">
       <c r="E19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>246</v>
+      </c>
       <c r="H19" s="30" t="s">
         <v>60</v>
       </c>

</xml_diff>